<commit_message>
finish backend fixes, start ui
</commit_message>
<xml_diff>
--- a/latin_input_v4.xlsx
+++ b/latin_input_v4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5f66ddf2985e7d8/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="763" documentId="8_{A460020E-9B81-4DEB-8873-0C42BE60C496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98B8FEBB-EED5-4BCB-BDF9-315D87A19AC8}"/>
+  <xr:revisionPtr revIDLastSave="944" documentId="8_{A460020E-9B81-4DEB-8873-0C42BE60C496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CA1673E-7393-4F25-A807-F99EC9B76A34}"/>
   <bookViews>
     <workbookView xWindow="1410" yWindow="370" windowWidth="17590" windowHeight="9660" xr2:uid="{B5A39C7D-0FAA-420D-AEB3-44FB0F1CC1EB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="710">
   <si>
     <t>avoir</t>
   </si>
@@ -1841,9 +1841,6 @@
     <t>foie</t>
   </si>
   <si>
-    <t>éclair</t>
-  </si>
-  <si>
     <t>voleur</t>
   </si>
   <si>
@@ -1866,6 +1863,309 @@
   </si>
   <si>
     <t xml:space="preserve">caput, capitis, n. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nomina en 'en' </t>
+  </si>
+  <si>
+    <t>nomen</t>
+  </si>
+  <si>
+    <t>nom</t>
+  </si>
+  <si>
+    <t>cognomen</t>
+  </si>
+  <si>
+    <t>nom de famille</t>
+  </si>
+  <si>
+    <t>praenomen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prénom </t>
+  </si>
+  <si>
+    <t>volumen</t>
+  </si>
+  <si>
+    <t>livre</t>
+  </si>
+  <si>
+    <t>fulmen</t>
+  </si>
+  <si>
+    <t>foudre</t>
+  </si>
+  <si>
+    <t>flumen</t>
+  </si>
+  <si>
+    <t>rivière</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nomina en 'ens' </t>
+  </si>
+  <si>
+    <t>cliens</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>dens</t>
+  </si>
+  <si>
+    <t>dent</t>
+  </si>
+  <si>
+    <t>oriens</t>
+  </si>
+  <si>
+    <t>est</t>
+  </si>
+  <si>
+    <t>occidens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ouest </t>
+  </si>
+  <si>
+    <t>frons</t>
+  </si>
+  <si>
+    <t>front</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mons </t>
+  </si>
+  <si>
+    <t>montagne</t>
+  </si>
+  <si>
+    <t>pons</t>
+  </si>
+  <si>
+    <t>pont</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nomina en 'ons' </t>
+  </si>
+  <si>
+    <t>miles</t>
+  </si>
+  <si>
+    <t>soldat</t>
+  </si>
+  <si>
+    <t>comes</t>
+  </si>
+  <si>
+    <t>associé</t>
+  </si>
+  <si>
+    <t>vates</t>
+  </si>
+  <si>
+    <t>prophète</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pes </t>
+  </si>
+  <si>
+    <t>nubes</t>
+  </si>
+  <si>
+    <t>eques</t>
+  </si>
+  <si>
+    <t>pied</t>
+  </si>
+  <si>
+    <t>nuage</t>
+  </si>
+  <si>
+    <t>pedes</t>
+  </si>
+  <si>
+    <t>cavalier</t>
+  </si>
+  <si>
+    <t>piéton</t>
+  </si>
+  <si>
+    <t>dies</t>
+  </si>
+  <si>
+    <t>jour</t>
+  </si>
+  <si>
+    <t>glacies</t>
+  </si>
+  <si>
+    <t>glacier</t>
+  </si>
+  <si>
+    <t>res</t>
+  </si>
+  <si>
+    <t>chose</t>
+  </si>
+  <si>
+    <t>vox</t>
+  </si>
+  <si>
+    <t>voix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nomina en 'ox' </t>
+  </si>
+  <si>
+    <t>sacerdos</t>
+  </si>
+  <si>
+    <t>prêtre</t>
+  </si>
+  <si>
+    <t>mos</t>
+  </si>
+  <si>
+    <t>moeurs</t>
+  </si>
+  <si>
+    <t>os</t>
+  </si>
+  <si>
+    <t>bouche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nomina en 'os' </t>
+  </si>
+  <si>
+    <t>uxor</t>
+  </si>
+  <si>
+    <t>épouse</t>
+  </si>
+  <si>
+    <t>soror</t>
+  </si>
+  <si>
+    <t>soeur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratiocinator </t>
+  </si>
+  <si>
+    <t>comptable</t>
+  </si>
+  <si>
+    <t>pictor</t>
+  </si>
+  <si>
+    <t>peintre</t>
+  </si>
+  <si>
+    <t>pistor</t>
+  </si>
+  <si>
+    <t>boulanger</t>
+  </si>
+  <si>
+    <t>mercator</t>
+  </si>
+  <si>
+    <t>marchand</t>
+  </si>
+  <si>
+    <t>professor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">professeur </t>
+  </si>
+  <si>
+    <t>gladiator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gladiateur </t>
+  </si>
+  <si>
+    <t>orator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orateur </t>
+  </si>
+  <si>
+    <t>emptor</t>
+  </si>
+  <si>
+    <t>acheteur</t>
+  </si>
+  <si>
+    <t>arbor</t>
+  </si>
+  <si>
+    <t>arbre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pastor </t>
+  </si>
+  <si>
+    <t>berger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timor </t>
+  </si>
+  <si>
+    <t>crainte</t>
+  </si>
+  <si>
+    <t>clamor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cri </t>
+  </si>
+  <si>
+    <t>cor</t>
+  </si>
+  <si>
+    <t>coeur</t>
+  </si>
+  <si>
+    <t>gubernator</t>
+  </si>
+  <si>
+    <t>captaine de bateau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nomina en 'or' </t>
+  </si>
+  <si>
+    <t>vesper</t>
+  </si>
+  <si>
+    <t>soir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vesper, vesperis, m. </t>
+  </si>
+  <si>
+    <t>iter</t>
+  </si>
+  <si>
+    <t>voyage</t>
+  </si>
+  <si>
+    <t>pater</t>
+  </si>
+  <si>
+    <t>père</t>
+  </si>
+  <si>
+    <t>portus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">port </t>
   </si>
 </sst>
 </file>
@@ -1881,12 +2181,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1901,7 +2207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1911,6 +2217,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2250,10 +2559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F55555-A930-445C-ABBA-239A271FB196}">
-  <dimension ref="A1:H304"/>
+  <dimension ref="A1:H351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="G169" sqref="G169"/>
+    <sheetView tabSelected="1" topLeftCell="A349" workbookViewId="0">
+      <selection activeCell="E212" sqref="E212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4331,13 +4640,13 @@
         <v>3</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>13</v>
+        <v>612</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>3</v>
+        <v>613</v>
       </c>
       <c r="H147" t="s">
-        <v>591</v>
+        <v>609</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.35">
@@ -4348,13 +4657,10 @@
         <v>3</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>12</v>
+        <v>618</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H148" t="s">
-        <v>590</v>
+        <v>619</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.35">
@@ -4365,16 +4671,10 @@
         <v>3</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>571</v>
+        <v>620</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="E149" s="2" t="s">
-        <v>573</v>
-      </c>
-      <c r="H149" t="s">
-        <v>589</v>
+        <v>621</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.35">
@@ -4385,13 +4685,10 @@
         <v>3</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>557</v>
+        <v>610</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>558</v>
-      </c>
-      <c r="E150" s="2" t="s">
-        <v>565</v>
+        <v>611</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.35">
@@ -4402,13 +4699,10 @@
         <v>3</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>586</v>
+        <v>614</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>587</v>
-      </c>
-      <c r="E151" s="2" t="s">
-        <v>588</v>
+        <v>615</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.35">
@@ -4419,13 +4713,10 @@
         <v>3</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>577</v>
+        <v>616</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>578</v>
-      </c>
-      <c r="E152" s="2" t="s">
-        <v>579</v>
+        <v>617</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.35">
@@ -4436,13 +4727,13 @@
         <v>3</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>552</v>
+        <v>623</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="E153" s="2" t="s">
-        <v>563</v>
+        <v>624</v>
+      </c>
+      <c r="H153" t="s">
+        <v>622</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.35">
@@ -4453,13 +4744,10 @@
         <v>3</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>574</v>
+        <v>625</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>575</v>
-      </c>
-      <c r="E154" s="2" t="s">
-        <v>576</v>
+        <v>626</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.35">
@@ -4470,13 +4758,10 @@
         <v>3</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>568</v>
+        <v>629</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>569</v>
-      </c>
-      <c r="E155" s="2" t="s">
-        <v>570</v>
+        <v>630</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.35">
@@ -4487,13 +4772,10 @@
         <v>3</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>561</v>
+        <v>627</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="E156" s="2" t="s">
-        <v>567</v>
+        <v>628</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.35">
@@ -4504,13 +4786,10 @@
         <v>3</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>580</v>
+        <v>704</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="E157" s="2" t="s">
-        <v>582</v>
+        <v>705</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.35">
@@ -4521,13 +4800,13 @@
         <v>3</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>559</v>
+        <v>13</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>560</v>
-      </c>
-      <c r="E158" s="2" t="s">
-        <v>566</v>
+        <v>3</v>
+      </c>
+      <c r="H158" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.35">
@@ -4538,13 +4817,10 @@
         <v>3</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>583</v>
+        <v>706</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>584</v>
-      </c>
-      <c r="E159" s="2" t="s">
-        <v>585</v>
+        <v>707</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.35">
@@ -4555,13 +4831,13 @@
         <v>3</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>554</v>
+        <v>701</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>555</v>
+        <v>702</v>
       </c>
       <c r="E160" s="2" t="s">
-        <v>564</v>
+        <v>703</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.35">
@@ -4572,13 +4848,10 @@
         <v>3</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>554</v>
+        <v>640</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="E161" s="2" t="s">
-        <v>564</v>
+        <v>641</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.35">
@@ -4589,16 +4862,10 @@
         <v>3</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>593</v>
+        <v>646</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>594</v>
-      </c>
-      <c r="E162" s="2" t="s">
-        <v>595</v>
-      </c>
-      <c r="H162" t="s">
-        <v>596</v>
+        <v>650</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.35">
@@ -4609,16 +4876,10 @@
         <v>3</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>598</v>
+        <v>638</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>601</v>
-      </c>
-      <c r="E163" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="H163" t="s">
-        <v>592</v>
+        <v>639</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.35">
@@ -4629,13 +4890,10 @@
         <v>3</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>597</v>
+        <v>645</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>602</v>
-      </c>
-      <c r="E164" s="2" t="s">
-        <v>604</v>
+        <v>648</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.35">
@@ -4645,14 +4903,11 @@
       <c r="B165" s="1">
         <v>3</v>
       </c>
-      <c r="C165" s="1" t="s">
-        <v>599</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>600</v>
-      </c>
-      <c r="E165" s="2" t="s">
-        <v>605</v>
+      <c r="C165" s="4" t="s">
+        <v>649</v>
+      </c>
+      <c r="D165" s="4" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.35">
@@ -4663,16 +4918,10 @@
         <v>3</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>607</v>
+        <v>644</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>608</v>
-      </c>
-      <c r="E166" s="2" t="s">
-        <v>609</v>
-      </c>
-      <c r="H166" t="s">
-        <v>606</v>
+        <v>647</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.35">
@@ -4680,13 +4929,13 @@
         <v>2</v>
       </c>
       <c r="B167" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>26</v>
+        <v>642</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>27</v>
+        <v>643</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.35">
@@ -4694,797 +4943,878 @@
         <v>2</v>
       </c>
       <c r="B168" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>29</v>
+        <v>8</v>
+      </c>
+      <c r="H168" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B169" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>361</v>
+        <v>571</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>362</v>
+        <v>572</v>
+      </c>
+      <c r="E169" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="H169" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B170" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>376</v>
+        <v>557</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>481</v>
+        <v>558</v>
+      </c>
+      <c r="E170" s="2" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B171" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>377</v>
+        <v>586</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>378</v>
+        <v>587</v>
+      </c>
+      <c r="E171" s="2" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A172" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B172" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>365</v>
+        <v>577</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>366</v>
+        <v>578</v>
+      </c>
+      <c r="E172" s="2" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B173" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>363</v>
+        <v>552</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>364</v>
+        <v>553</v>
+      </c>
+      <c r="E173" s="2" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B174" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>367</v>
+        <v>574</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>368</v>
+        <v>575</v>
+      </c>
+      <c r="E174" s="2" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A175" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B175" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>369</v>
+        <v>568</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>370</v>
+        <v>569</v>
+      </c>
+      <c r="E175" s="2" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A176" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B176" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C176" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="E176" s="2" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A177" s="1">
+        <v>2</v>
+      </c>
+      <c r="B177" s="1">
+        <v>3</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A178" s="1">
+        <v>2</v>
+      </c>
+      <c r="B178" s="1">
+        <v>3</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A179" s="1">
+        <v>2</v>
+      </c>
+      <c r="B179" s="1">
+        <v>3</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="E179" s="2" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A180" s="1">
+        <v>2</v>
+      </c>
+      <c r="B180" s="1">
+        <v>3</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="E180" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A181" s="1">
+        <v>2</v>
+      </c>
+      <c r="B181" s="1">
+        <v>3</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="E181" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A182" s="1">
+        <v>2</v>
+      </c>
+      <c r="B182" s="1">
+        <v>3</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="H182" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A183" s="1">
+        <v>2</v>
+      </c>
+      <c r="B183" s="1">
+        <v>3</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A184" s="1">
+        <v>2</v>
+      </c>
+      <c r="B184" s="1">
+        <v>3</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A185" s="1">
+        <v>2</v>
+      </c>
+      <c r="B185" s="1">
+        <v>3</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="H185" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A186" s="1">
+        <v>2</v>
+      </c>
+      <c r="B186" s="1">
+        <v>3</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A187" s="1">
+        <v>2</v>
+      </c>
+      <c r="B187" s="1">
+        <v>3</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A188" s="1">
+        <v>2</v>
+      </c>
+      <c r="B188" s="1">
+        <v>3</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A189" s="1">
+        <v>2</v>
+      </c>
+      <c r="B189" s="1">
+        <v>3</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A190" s="1">
+        <v>2</v>
+      </c>
+      <c r="B190" s="1">
+        <v>3</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A191" s="1">
+        <v>2</v>
+      </c>
+      <c r="B191" s="1">
+        <v>3</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A192" s="1">
+        <v>2</v>
+      </c>
+      <c r="B192" s="1">
+        <v>3</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A193" s="1">
+        <v>2</v>
+      </c>
+      <c r="B193" s="1">
+        <v>3</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A194" s="1">
+        <v>2</v>
+      </c>
+      <c r="B194" s="1">
+        <v>3</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A195" s="1">
+        <v>2</v>
+      </c>
+      <c r="B195" s="1">
+        <v>3</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A196" s="1">
+        <v>2</v>
+      </c>
+      <c r="B196" s="1">
+        <v>3</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A197" s="1">
+        <v>2</v>
+      </c>
+      <c r="B197" s="1">
+        <v>3</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A198" s="1">
+        <v>2</v>
+      </c>
+      <c r="B198" s="1">
+        <v>3</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A199" s="1">
+        <v>2</v>
+      </c>
+      <c r="B199" s="1">
+        <v>3</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A200" s="1">
+        <v>2</v>
+      </c>
+      <c r="B200" s="1">
+        <v>3</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A201" s="1">
+        <v>2</v>
+      </c>
+      <c r="B201" s="1">
+        <v>3</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="H201" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A202" s="1">
+        <v>2</v>
+      </c>
+      <c r="B202" s="1">
+        <v>3</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A203" s="1">
+        <v>2</v>
+      </c>
+      <c r="B203" s="1">
+        <v>3</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A204" s="1">
+        <v>2</v>
+      </c>
+      <c r="B204" s="1">
+        <v>3</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="H204" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A205" s="1">
+        <v>2</v>
+      </c>
+      <c r="B205" s="1">
+        <v>3</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="E205" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="H205" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A206" s="1">
+        <v>2</v>
+      </c>
+      <c r="B206" s="1">
+        <v>3</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="D206" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="E206" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="H206" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A207" s="1">
+        <v>2</v>
+      </c>
+      <c r="B207" s="1">
+        <v>3</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="E207" s="2" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A208" s="1">
+        <v>2</v>
+      </c>
+      <c r="B208" s="1">
+        <v>3</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="E208" s="2" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A209" s="1">
+        <v>2</v>
+      </c>
+      <c r="B209" s="1">
+        <v>3</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="E209" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="H209" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A210" s="1">
+        <v>2</v>
+      </c>
+      <c r="B210" s="1">
+        <v>4</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A211" s="1">
+        <v>2</v>
+      </c>
+      <c r="B211" s="1">
+        <v>5</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A212" s="1">
+        <v>2</v>
+      </c>
+      <c r="B212" s="1">
+        <v>5</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A213" s="1">
+        <v>2</v>
+      </c>
+      <c r="B213" s="1">
+        <v>5</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A214" s="1">
+        <v>2</v>
+      </c>
+      <c r="B214" s="1">
+        <v>5</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A215" s="1">
+        <v>2</v>
+      </c>
+      <c r="B215" s="1">
+        <v>5</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A216" s="1">
+        <v>3</v>
+      </c>
+      <c r="B216" s="1">
+        <v>1</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A217" s="1">
+        <v>3</v>
+      </c>
+      <c r="B217" s="1">
+        <v>1</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A218" s="1">
+        <v>3</v>
+      </c>
+      <c r="B218" s="1">
+        <v>1</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A219" s="1">
+        <v>3</v>
+      </c>
+      <c r="B219" s="1">
+        <v>1</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A220" s="1">
+        <v>3</v>
+      </c>
+      <c r="B220" s="1">
+        <v>1</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A221" s="1">
+        <v>3</v>
+      </c>
+      <c r="B221" s="1">
+        <v>1</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A222" s="1">
+        <v>3</v>
+      </c>
+      <c r="B222" s="1">
+        <v>1</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A223" s="1">
+        <v>3</v>
+      </c>
+      <c r="B223" s="1">
+        <v>1</v>
+      </c>
+      <c r="C223" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="D176" s="1" t="s">
+      <c r="D223" s="1" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A177" s="1">
-        <v>3</v>
-      </c>
-      <c r="B177" s="1">
-        <v>1</v>
-      </c>
-      <c r="C177" s="1" t="s">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A224" s="1">
+        <v>3</v>
+      </c>
+      <c r="B224" s="1">
+        <v>1</v>
+      </c>
+      <c r="C224" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="D177" s="1" t="s">
+      <c r="D224" s="1" t="s">
         <v>374</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A178" s="1">
-        <v>3</v>
-      </c>
-      <c r="B178" s="1">
-        <v>1</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="D178" s="1" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A179" s="1">
-        <v>3</v>
-      </c>
-      <c r="B179" s="1">
-        <v>1</v>
-      </c>
-      <c r="C179" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="D179" s="1" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A180" s="1">
-        <v>3</v>
-      </c>
-      <c r="B180" s="1">
-        <v>1</v>
-      </c>
-      <c r="C180" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="D180" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A181" s="1">
-        <v>3</v>
-      </c>
-      <c r="B181" s="1">
-        <v>1</v>
-      </c>
-      <c r="C181" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="D181" s="1" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A182" s="1">
-        <v>3</v>
-      </c>
-      <c r="B182" s="1">
-        <v>1</v>
-      </c>
-      <c r="C182" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D182" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A183" s="1">
-        <v>3</v>
-      </c>
-      <c r="B183" s="1">
-        <v>1</v>
-      </c>
-      <c r="C183" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="D183" s="1" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A184" s="1">
-        <v>3</v>
-      </c>
-      <c r="B184" s="1">
-        <v>1</v>
-      </c>
-      <c r="C184" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="D184" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A185" s="1">
-        <v>3</v>
-      </c>
-      <c r="B185" s="1">
-        <v>1</v>
-      </c>
-      <c r="C185" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="D185" s="1" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A186" s="1">
-        <v>3</v>
-      </c>
-      <c r="B186" s="1">
-        <v>1</v>
-      </c>
-      <c r="C186" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="D186" s="1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A187" s="1">
-        <v>3</v>
-      </c>
-      <c r="B187" s="1">
-        <v>1</v>
-      </c>
-      <c r="C187" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="D187" s="1" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A188" s="1">
-        <v>3</v>
-      </c>
-      <c r="B188" s="1">
-        <v>1</v>
-      </c>
-      <c r="C188" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="D188" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A189" s="1">
-        <v>3</v>
-      </c>
-      <c r="B189" s="1">
-        <v>1</v>
-      </c>
-      <c r="C189" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="D189" s="1" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A190" s="1">
-        <v>3</v>
-      </c>
-      <c r="B190" s="1">
-        <v>1</v>
-      </c>
-      <c r="C190" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="D190" s="1" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A191" s="1">
-        <v>3</v>
-      </c>
-      <c r="B191" s="1">
-        <v>1</v>
-      </c>
-      <c r="C191" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D191" s="1" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A192" s="1">
-        <v>3</v>
-      </c>
-      <c r="B192" s="1">
-        <v>1</v>
-      </c>
-      <c r="C192" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="D192" s="1" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A193" s="1">
-        <v>3</v>
-      </c>
-      <c r="B193" s="1">
-        <v>1</v>
-      </c>
-      <c r="C193" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="D193" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A194" s="1">
-        <v>3</v>
-      </c>
-      <c r="B194" s="1">
-        <v>1</v>
-      </c>
-      <c r="C194" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="D194" s="1" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A195" s="1">
-        <v>3</v>
-      </c>
-      <c r="B195" s="1">
-        <v>1</v>
-      </c>
-      <c r="C195" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="D195" s="1" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A196" s="1">
-        <v>3</v>
-      </c>
-      <c r="B196" s="1">
-        <v>1</v>
-      </c>
-      <c r="C196" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="D196" s="1" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A197" s="1">
-        <v>3</v>
-      </c>
-      <c r="B197" s="1">
-        <v>1</v>
-      </c>
-      <c r="C197" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="D197" s="1" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A198" s="1">
-        <v>3</v>
-      </c>
-      <c r="B198" s="1">
-        <v>1</v>
-      </c>
-      <c r="C198" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="D198" s="1" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A199" s="1">
-        <v>3</v>
-      </c>
-      <c r="B199" s="1">
-        <v>1</v>
-      </c>
-      <c r="C199" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="D199" s="1" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A200" s="1">
-        <v>3</v>
-      </c>
-      <c r="B200" s="1">
-        <v>1</v>
-      </c>
-      <c r="C200" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="D200" s="1" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A201" s="1">
-        <v>3</v>
-      </c>
-      <c r="B201" s="1">
-        <v>1</v>
-      </c>
-      <c r="C201" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="D201" s="1" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A202" s="1">
-        <v>3</v>
-      </c>
-      <c r="B202" s="1">
-        <v>1</v>
-      </c>
-      <c r="C202" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="D202" s="1" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A203" s="1">
-        <v>3</v>
-      </c>
-      <c r="B203" s="1">
-        <v>1</v>
-      </c>
-      <c r="C203" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="D203" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A204" s="1">
-        <v>3</v>
-      </c>
-      <c r="B204" s="1">
-        <v>1</v>
-      </c>
-      <c r="C204" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="D204" s="1" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A205" s="1">
-        <v>3</v>
-      </c>
-      <c r="B205" s="1">
-        <v>1</v>
-      </c>
-      <c r="C205" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="D205" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A206" s="1">
-        <v>3</v>
-      </c>
-      <c r="B206" s="1">
-        <v>1</v>
-      </c>
-      <c r="C206" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="D206" s="1" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A207" s="1">
-        <v>3</v>
-      </c>
-      <c r="B207" s="1">
-        <v>1</v>
-      </c>
-      <c r="C207" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="D207" s="1" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A208" s="1">
-        <v>3</v>
-      </c>
-      <c r="B208" s="1">
-        <v>1</v>
-      </c>
-      <c r="C208" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="D208" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A209" s="1">
-        <v>3</v>
-      </c>
-      <c r="B209" s="1">
-        <v>1</v>
-      </c>
-      <c r="C209" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="D209" s="1" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A210" s="1">
-        <v>3</v>
-      </c>
-      <c r="B210" s="1">
-        <v>1</v>
-      </c>
-      <c r="C210" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="D210" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A211" s="1">
-        <v>3</v>
-      </c>
-      <c r="B211" s="1">
-        <v>1</v>
-      </c>
-      <c r="C211" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="D211" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A212" s="1">
-        <v>3</v>
-      </c>
-      <c r="B212" s="1">
-        <v>1</v>
-      </c>
-      <c r="C212" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="D212" s="1" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A213" s="1">
-        <v>3</v>
-      </c>
-      <c r="B213" s="1">
-        <v>1</v>
-      </c>
-      <c r="C213" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="D213" s="1" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A214" s="1">
-        <v>3</v>
-      </c>
-      <c r="B214" s="1">
-        <v>1</v>
-      </c>
-      <c r="C214" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="D214" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A215" s="1">
-        <v>3</v>
-      </c>
-      <c r="B215" s="1">
-        <v>1</v>
-      </c>
-      <c r="C215" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="D215" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A216" s="1">
-        <v>3</v>
-      </c>
-      <c r="B216" s="1">
-        <v>1</v>
-      </c>
-      <c r="C216" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="D216" s="1" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A217" s="1">
-        <v>3</v>
-      </c>
-      <c r="B217" s="1">
-        <v>1</v>
-      </c>
-      <c r="C217" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="D217" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A218" s="1">
-        <v>3</v>
-      </c>
-      <c r="B218" s="1">
-        <v>1</v>
-      </c>
-      <c r="C218" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="D218" s="1" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A219" s="1">
-        <v>3</v>
-      </c>
-      <c r="B219" s="1">
-        <v>1</v>
-      </c>
-      <c r="C219" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="D219" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A220" s="1">
-        <v>3</v>
-      </c>
-      <c r="B220" s="1">
-        <v>1</v>
-      </c>
-      <c r="C220" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="D220" s="1" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A221" s="1">
-        <v>3</v>
-      </c>
-      <c r="B221" s="1">
-        <v>1</v>
-      </c>
-      <c r="C221" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="D221" s="1" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A222" s="1">
-        <v>3</v>
-      </c>
-      <c r="B222" s="1">
-        <v>1</v>
-      </c>
-      <c r="C222" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="D222" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A223" s="1">
-        <v>3</v>
-      </c>
-      <c r="B223" s="1">
-        <v>1</v>
-      </c>
-      <c r="C223" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="D223" s="1" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A224" s="1">
-        <v>3</v>
-      </c>
-      <c r="B224" s="1">
-        <v>1</v>
-      </c>
-      <c r="C224" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="D224" s="1" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.35">
@@ -5495,10 +5825,10 @@
         <v>1</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>473</v>
+        <v>379</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>496</v>
+        <v>380</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.35">
@@ -5509,10 +5839,10 @@
         <v>1</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>426</v>
+        <v>375</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>427</v>
+        <v>482</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.35">
@@ -5523,10 +5853,10 @@
         <v>1</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>433</v>
+        <v>382</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>497</v>
+        <v>383</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.35">
@@ -5537,10 +5867,10 @@
         <v>1</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>436</v>
+        <v>381</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>437</v>
+        <v>483</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.35">
@@ -5551,10 +5881,10 @@
         <v>1</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>475</v>
+        <v>11</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>498</v>
+        <v>2</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.35">
@@ -5565,10 +5895,10 @@
         <v>1</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>444</v>
+        <v>411</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>499</v>
+        <v>412</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.35">
@@ -5579,10 +5909,10 @@
         <v>1</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>422</v>
+        <v>456</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>423</v>
+        <v>457</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.35">
@@ -5593,10 +5923,10 @@
         <v>1</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>414</v>
+        <v>484</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.35">
@@ -5607,10 +5937,10 @@
         <v>1</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>466</v>
+        <v>450</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.35">
@@ -5621,10 +5951,10 @@
         <v>1</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>454</v>
+        <v>485</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.35">
@@ -5635,10 +5965,10 @@
         <v>1</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>434</v>
+        <v>445</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>435</v>
+        <v>383</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.35">
@@ -5649,10 +5979,10 @@
         <v>1</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>467</v>
+        <v>418</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>468</v>
+        <v>486</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.35">
@@ -5663,10 +5993,10 @@
         <v>1</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>395</v>
+        <v>478</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>396</v>
+        <v>479</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.35">
@@ -5677,10 +6007,10 @@
         <v>1</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>480</v>
+        <v>421</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>359</v>
+        <v>487</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.35">
@@ -5691,10 +6021,10 @@
         <v>1</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>440</v>
+        <v>474</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>441</v>
+        <v>488</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.35">
@@ -5705,966 +6035,1624 @@
         <v>1</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>469</v>
+        <v>400</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A241" s="1">
         <v>3</v>
       </c>
       <c r="B241" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>347</v>
+        <v>477</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A242" s="1">
         <v>3</v>
       </c>
       <c r="B242" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>346</v>
+        <v>463</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A243" s="1">
         <v>3</v>
       </c>
       <c r="B243" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>352</v>
+        <v>458</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A244" s="1">
         <v>3</v>
       </c>
       <c r="B244" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>348</v>
+        <v>384</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A245" s="1">
         <v>3</v>
       </c>
       <c r="B245" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>358</v>
+        <v>409</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A246" s="1">
         <v>3</v>
       </c>
       <c r="B246" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>15</v>
+        <v>447</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A247" s="1">
         <v>3</v>
       </c>
       <c r="B247" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>356</v>
+        <v>446</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A248" s="1">
         <v>3</v>
       </c>
       <c r="B248" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A249" s="1">
         <v>3</v>
       </c>
       <c r="B249" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>354</v>
+        <v>428</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A250" s="1">
         <v>3</v>
       </c>
       <c r="B250" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>17</v>
+        <v>391</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A251" s="1">
         <v>3</v>
       </c>
       <c r="B251" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>350</v>
+        <v>407</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A252" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B252" s="1">
         <v>1</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>44</v>
+        <v>405</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E252" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A253" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B253" s="1">
         <v>1</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>44</v>
+        <v>385</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E253" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A254" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B254" s="1">
         <v>1</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>323</v>
+        <v>451</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E254" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A255" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B255" s="1">
         <v>1</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>209</v>
+        <v>460</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E255" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A256" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B256" s="1">
         <v>1</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>342</v>
+        <v>471</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="E256" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A257" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B257" s="1">
         <v>1</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>336</v>
+        <v>431</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="E257" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A258" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B258" s="1">
         <v>1</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>338</v>
+        <v>398</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="E258" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A259" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B259" s="1">
         <v>1</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>207</v>
+        <v>419</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E259" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A260" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B260" s="1">
         <v>1</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>214</v>
+        <v>438</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E260" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A261" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B261" s="1">
         <v>1</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>195</v>
+        <v>397</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E261" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A262" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B262" s="1">
         <v>1</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>199</v>
+        <v>416</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="E262" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A263" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B263" s="1">
         <v>1</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>340</v>
+        <v>432</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="E263" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A264" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B264" s="1">
         <v>1</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>204</v>
+        <v>424</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="E264" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A265" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B265" s="1">
         <v>1</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>327</v>
+        <v>402</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="E265" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A266" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B266" s="1">
         <v>1</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>331</v>
+        <v>404</v>
       </c>
       <c r="D266" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="E266" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A267" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B267" s="1">
         <v>1</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>211</v>
+        <v>462</v>
       </c>
       <c r="D267" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="E267" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A268" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B268" s="1">
         <v>1</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>206</v>
+        <v>389</v>
       </c>
       <c r="D268" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E268" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A269" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B269" s="1">
         <v>1</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>503</v>
+        <v>393</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="E269" s="3"/>
-    </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A270" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B270" s="1">
         <v>1</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>333</v>
+        <v>442</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="E270" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A271" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B271" s="1">
         <v>1</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>325</v>
+        <v>430</v>
       </c>
       <c r="D271" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="E271" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A272" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B272" s="1">
         <v>1</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>329</v>
+        <v>473</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="E272" s="3" t="s">
-        <v>203</v>
+        <v>496</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A273" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B273" s="1">
         <v>1</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>197</v>
+        <v>426</v>
       </c>
       <c r="D273" s="1" t="s">
-        <v>200</v>
+        <v>427</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A274" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B274" s="1">
         <v>1</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>198</v>
+        <v>433</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>201</v>
+        <v>497</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A275" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B275" s="1">
         <v>1</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>510</v>
+        <v>436</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>509</v>
+        <v>437</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A276" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B276" s="1">
         <v>1</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>532</v>
+        <v>475</v>
       </c>
       <c r="D276" s="1" t="s">
-        <v>533</v>
+        <v>498</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A277" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B277" s="1">
         <v>1</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>207</v>
+        <v>444</v>
       </c>
       <c r="D277" s="1" t="s">
-        <v>551</v>
+        <v>499</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A278" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B278" s="1">
         <v>1</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>549</v>
+        <v>422</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>550</v>
+        <v>423</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A279" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B279" s="1">
         <v>1</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>528</v>
+        <v>413</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>527</v>
+        <v>414</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A280" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B280" s="1">
         <v>1</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>513</v>
+        <v>465</v>
       </c>
       <c r="D280" s="1" t="s">
-        <v>514</v>
+        <v>466</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A281" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B281" s="1">
         <v>1</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>501</v>
+        <v>453</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>502</v>
+        <v>454</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A282" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B282" s="1">
         <v>1</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>534</v>
+        <v>434</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>535</v>
+        <v>435</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A283" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B283" s="1">
         <v>1</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>531</v>
+        <v>467</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>530</v>
+        <v>468</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A284" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B284" s="1">
         <v>1</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>504</v>
+        <v>395</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>505</v>
+        <v>396</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A285" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B285" s="1">
         <v>1</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>518</v>
+        <v>480</v>
       </c>
       <c r="D285" s="1" t="s">
-        <v>519</v>
+        <v>359</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A286" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B286" s="1">
         <v>1</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>536</v>
+        <v>440</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>537</v>
+        <v>441</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A287" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B287" s="1">
         <v>1</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>507</v>
+        <v>469</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>508</v>
+        <v>470</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A288" s="1">
+        <v>3</v>
+      </c>
+      <c r="B288" s="1">
+        <v>3</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D288" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A289" s="1">
+        <v>3</v>
+      </c>
+      <c r="B289" s="1">
+        <v>3</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D289" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A290" s="1">
+        <v>3</v>
+      </c>
+      <c r="B290" s="1">
+        <v>3</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D290" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A291" s="1">
+        <v>3</v>
+      </c>
+      <c r="B291" s="1">
+        <v>3</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D291" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A292" s="1">
+        <v>3</v>
+      </c>
+      <c r="B292" s="1">
+        <v>3</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="D292" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A293" s="1">
+        <v>3</v>
+      </c>
+      <c r="B293" s="1">
+        <v>3</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D293" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B288" s="1">
-        <v>1</v>
-      </c>
-      <c r="C288" s="1" t="s">
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A294" s="1">
+        <v>3</v>
+      </c>
+      <c r="B294" s="1">
+        <v>3</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D294" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A295" s="1">
+        <v>3</v>
+      </c>
+      <c r="B295" s="1">
+        <v>3</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D295" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A296" s="1">
+        <v>3</v>
+      </c>
+      <c r="B296" s="1">
+        <v>3</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D296" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A297" s="1">
+        <v>3</v>
+      </c>
+      <c r="B297" s="1">
+        <v>3</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D297" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A298" s="1">
+        <v>3</v>
+      </c>
+      <c r="B298" s="1">
+        <v>3</v>
+      </c>
+      <c r="C298" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="D298" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A299" s="1">
+        <v>4</v>
+      </c>
+      <c r="B299" s="1">
+        <v>1</v>
+      </c>
+      <c r="C299" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D299" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E299" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A300" s="1">
+        <v>4</v>
+      </c>
+      <c r="B300" s="1">
+        <v>1</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D300" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E300" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A301" s="1">
+        <v>4</v>
+      </c>
+      <c r="B301" s="1">
+        <v>1</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D301" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E301" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A302" s="1">
+        <v>4</v>
+      </c>
+      <c r="B302" s="1">
+        <v>1</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D302" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E302" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A303" s="1">
+        <v>4</v>
+      </c>
+      <c r="B303" s="1">
+        <v>1</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D303" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="E303" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A304" s="1">
+        <v>4</v>
+      </c>
+      <c r="B304" s="1">
+        <v>1</v>
+      </c>
+      <c r="C304" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D304" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="E304" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A305" s="1">
+        <v>4</v>
+      </c>
+      <c r="B305" s="1">
+        <v>1</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D305" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="E305" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A306" s="1">
+        <v>4</v>
+      </c>
+      <c r="B306" s="1">
+        <v>1</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D306" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E306" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A307" s="1">
+        <v>4</v>
+      </c>
+      <c r="B307" s="1">
+        <v>1</v>
+      </c>
+      <c r="C307" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D307" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E307" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A308" s="1">
+        <v>4</v>
+      </c>
+      <c r="B308" s="1">
+        <v>1</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D308" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E308" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A309" s="1">
+        <v>4</v>
+      </c>
+      <c r="B309" s="1">
+        <v>1</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D309" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E309" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A310" s="1">
+        <v>4</v>
+      </c>
+      <c r="B310" s="1">
+        <v>1</v>
+      </c>
+      <c r="C310" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D310" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E310" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A311" s="1">
+        <v>4</v>
+      </c>
+      <c r="B311" s="1">
+        <v>1</v>
+      </c>
+      <c r="C311" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D311" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E311" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A312" s="1">
+        <v>4</v>
+      </c>
+      <c r="B312" s="1">
+        <v>1</v>
+      </c>
+      <c r="C312" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D312" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E312" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A313" s="1">
+        <v>4</v>
+      </c>
+      <c r="B313" s="1">
+        <v>1</v>
+      </c>
+      <c r="C313" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D313" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="E313" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A314" s="1">
+        <v>4</v>
+      </c>
+      <c r="B314" s="1">
+        <v>1</v>
+      </c>
+      <c r="C314" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D314" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E314" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A315" s="1">
+        <v>4</v>
+      </c>
+      <c r="B315" s="1">
+        <v>1</v>
+      </c>
+      <c r="C315" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D315" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E315" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A316" s="1">
+        <v>4</v>
+      </c>
+      <c r="B316" s="1">
+        <v>1</v>
+      </c>
+      <c r="C316" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="D316" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E316" s="3"/>
+    </row>
+    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A317" s="1">
+        <v>4</v>
+      </c>
+      <c r="B317" s="1">
+        <v>1</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D317" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E317" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A318" s="1">
+        <v>4</v>
+      </c>
+      <c r="B318" s="1">
+        <v>1</v>
+      </c>
+      <c r="C318" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D318" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E318" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A319" s="1">
+        <v>4</v>
+      </c>
+      <c r="B319" s="1">
+        <v>1</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D319" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="E319" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A320" s="1">
+        <v>4</v>
+      </c>
+      <c r="B320" s="1">
+        <v>1</v>
+      </c>
+      <c r="C320" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D320" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A321" s="1">
+        <v>4</v>
+      </c>
+      <c r="B321" s="1">
+        <v>1</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D321" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A322" s="1">
+        <v>5</v>
+      </c>
+      <c r="B322" s="1">
+        <v>1</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="D322" s="1" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A323" s="1">
+        <v>5</v>
+      </c>
+      <c r="B323" s="1">
+        <v>1</v>
+      </c>
+      <c r="C323" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="D323" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A324" s="1">
+        <v>5</v>
+      </c>
+      <c r="B324" s="1">
+        <v>1</v>
+      </c>
+      <c r="C324" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D324" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A325" s="1">
+        <v>5</v>
+      </c>
+      <c r="B325" s="1">
+        <v>1</v>
+      </c>
+      <c r="C325" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="D325" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A326" s="1">
+        <v>5</v>
+      </c>
+      <c r="B326" s="1">
+        <v>1</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D326" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A327" s="1">
+        <v>5</v>
+      </c>
+      <c r="B327" s="1">
+        <v>1</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D327" s="1" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A328" s="1">
+        <v>5</v>
+      </c>
+      <c r="B328" s="1">
+        <v>1</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D328" s="1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A329" s="1">
+        <v>5</v>
+      </c>
+      <c r="B329" s="1">
+        <v>1</v>
+      </c>
+      <c r="C329" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="D329" s="1" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A330" s="1">
+        <v>5</v>
+      </c>
+      <c r="B330" s="1">
+        <v>1</v>
+      </c>
+      <c r="C330" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="D330" s="1" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A331" s="1">
+        <v>5</v>
+      </c>
+      <c r="B331" s="1">
+        <v>1</v>
+      </c>
+      <c r="C331" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="D331" s="1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A332" s="1">
+        <v>5</v>
+      </c>
+      <c r="B332" s="1">
+        <v>1</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D332" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A333" s="1">
+        <v>5</v>
+      </c>
+      <c r="B333" s="1">
+        <v>1</v>
+      </c>
+      <c r="C333" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="D333" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A334" s="1">
+        <v>5</v>
+      </c>
+      <c r="B334" s="1">
+        <v>1</v>
+      </c>
+      <c r="C334" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="D334" s="1" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A335" s="1">
+        <v>5</v>
+      </c>
+      <c r="B335" s="1">
+        <v>1</v>
+      </c>
+      <c r="C335" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="D288" s="1" t="s">
+      <c r="D335" s="1" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A289" s="1">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A336" s="1">
         <v>5</v>
       </c>
-      <c r="B289" s="1">
-        <v>1</v>
-      </c>
-      <c r="C289" s="1" t="s">
+      <c r="B336" s="1">
+        <v>1</v>
+      </c>
+      <c r="C336" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="D289" s="1" t="s">
+      <c r="D336" s="1" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A290" s="1">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A337" s="1">
         <v>5</v>
       </c>
-      <c r="B290" s="1">
-        <v>1</v>
-      </c>
-      <c r="C290" s="1" t="s">
+      <c r="B337" s="1">
+        <v>1</v>
+      </c>
+      <c r="C337" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="D290" s="1" t="s">
+      <c r="D337" s="1" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A291" s="1">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A338" s="1">
         <v>5</v>
       </c>
-      <c r="B291" s="1">
-        <v>1</v>
-      </c>
-      <c r="C291" s="1" t="s">
+      <c r="B338" s="1">
+        <v>1</v>
+      </c>
+      <c r="C338" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="D291" s="1" t="s">
+      <c r="D338" s="1" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A292" s="1">
+    <row r="339" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A339" s="1">
         <v>5</v>
       </c>
-      <c r="B292" s="1">
-        <v>1</v>
-      </c>
-      <c r="C292" s="1" t="s">
+      <c r="B339" s="1">
+        <v>1</v>
+      </c>
+      <c r="C339" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="D292" s="1" t="s">
+      <c r="D339" s="1" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A293" s="1">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A340" s="1">
         <v>5</v>
       </c>
-      <c r="B293" s="1">
-        <v>1</v>
-      </c>
-      <c r="C293" s="1" t="s">
+      <c r="B340" s="1">
+        <v>1</v>
+      </c>
+      <c r="C340" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="D293" s="1" t="s">
+      <c r="D340" s="1" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A294" s="1">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A341" s="1">
         <v>5</v>
       </c>
-      <c r="B294" s="1">
-        <v>1</v>
-      </c>
-      <c r="C294" s="1" t="s">
+      <c r="B341" s="1">
+        <v>1</v>
+      </c>
+      <c r="C341" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="D294" s="1" t="s">
+      <c r="D341" s="1" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A295" s="1">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A342" s="1">
         <v>5</v>
       </c>
-      <c r="B295" s="1">
-        <v>1</v>
-      </c>
-      <c r="C295" s="1" t="s">
+      <c r="B342" s="1">
+        <v>1</v>
+      </c>
+      <c r="C342" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="D295" s="1" t="s">
+      <c r="D342" s="1" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A296" s="1">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A343" s="1">
         <v>5</v>
       </c>
-      <c r="B296" s="1">
-        <v>1</v>
-      </c>
-      <c r="C296" s="1" t="s">
+      <c r="B343" s="1">
+        <v>1</v>
+      </c>
+      <c r="C343" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="D296" s="1" t="s">
+      <c r="D343" s="1" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A297" s="1">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A344" s="1">
         <v>5</v>
       </c>
-      <c r="B297" s="1">
-        <v>1</v>
-      </c>
-      <c r="C297" s="1" t="s">
+      <c r="B344" s="1">
+        <v>1</v>
+      </c>
+      <c r="C344" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="D297" s="1" t="s">
+      <c r="D344" s="1" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A298" s="1">
+    <row r="345" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A345" s="1">
         <v>5</v>
       </c>
-      <c r="B298" s="1">
-        <v>1</v>
-      </c>
-      <c r="C298" s="1" t="s">
+      <c r="B345" s="1">
+        <v>1</v>
+      </c>
+      <c r="C345" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="D298" s="1" t="s">
+      <c r="D345" s="1" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A299" s="1">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A346" s="1">
         <v>5</v>
       </c>
-      <c r="B299" s="1">
-        <v>1</v>
-      </c>
-      <c r="C299" s="1" t="s">
+      <c r="B346" s="1">
+        <v>1</v>
+      </c>
+      <c r="C346" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D299" s="1" t="s">
+      <c r="D346" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A300" s="1">
+    <row r="347" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A347" s="1">
         <v>5</v>
       </c>
-      <c r="B300" s="1">
-        <v>1</v>
-      </c>
-      <c r="C300" s="1" t="s">
+      <c r="B347" s="1">
+        <v>1</v>
+      </c>
+      <c r="C347" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="D300" s="1" t="s">
+      <c r="D347" s="1" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A301" s="1">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A348" s="1">
         <v>5</v>
       </c>
-      <c r="B301" s="1">
-        <v>1</v>
-      </c>
-      <c r="C301" s="1" t="s">
+      <c r="B348" s="1">
+        <v>1</v>
+      </c>
+      <c r="C348" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="D301" s="1" t="s">
+      <c r="D348" s="1" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A302" s="1">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A349" s="1">
         <v>5</v>
       </c>
-      <c r="B302" s="1">
-        <v>1</v>
-      </c>
-      <c r="C302" s="1" t="s">
+      <c r="B349" s="1">
+        <v>1</v>
+      </c>
+      <c r="C349" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="D302" s="1" t="s">
+      <c r="D349" s="1" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A303" s="1">
+    <row r="350" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A350" s="1">
         <v>5</v>
       </c>
-      <c r="B303" s="1">
-        <v>1</v>
-      </c>
-      <c r="C303" s="1" t="s">
+      <c r="B350" s="1">
+        <v>1</v>
+      </c>
+      <c r="C350" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="D303" s="1" t="s">
+      <c r="D350" s="1" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A304" s="1">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A351" s="1">
         <v>5</v>
       </c>
-      <c r="B304" s="1">
-        <v>1</v>
-      </c>
-      <c r="C304" s="1" t="s">
+      <c r="B351" s="1">
+        <v>1</v>
+      </c>
+      <c r="C351" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D304" s="1" t="s">
+      <c r="D351" s="1" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>